<commit_message>
addedd fixed issue of data revenue
</commit_message>
<xml_diff>
--- a/public/templates/Template_Revenue.xlsx
+++ b/public/templates/Template_Revenue.xlsx
@@ -32,10 +32,10 @@
     <t>bulan</t>
   </si>
   <si>
-    <t>ICHA NOVANIA</t>
-  </si>
-  <si>
-    <t>APIDT INFRASTRUCTURE</t>
+    <t>tio</t>
+  </si>
+  <si>
+    <t>TEL U</t>
   </si>
   <si>
     <t>01/2023</t>
@@ -419,7 +419,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="22.28" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>

</xml_diff>